<commit_message>
commit3- made some changes in Excel file.
</commit_message>
<xml_diff>
--- a/Compose Functionality of gmail Test Cases(Mannual).xlsx
+++ b/Compose Functionality of gmail Test Cases(Mannual).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sneha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sneha\ComposeFunctionalityTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E791EA-693C-491F-9583-AC95114F6BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20031771-8BD1-446E-8E49-8EC0F6483E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E5A1800D-6638-40EA-B614-550D860290C2}"/>
   </bookViews>
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,9 +333,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -697,7 +694,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,240 +708,240 @@
     <col min="7" max="7" width="13.54296875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="12" customFormat="1" ht="37" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>44175</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="93" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="93" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="62" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:8" ht="170.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:8" ht="186" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="93" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>

</xml_diff>